<commit_message>
fix: export pdf and excel laporan stok (point 5)
</commit_message>
<xml_diff>
--- a/public/export_template/template_stok.xlsx
+++ b/public/export_template/template_stok.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\BDR-PENJUALAN\public\export_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF4D11C-F7D5-4505-85D4-AB879F7BB958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F48BA9-97F8-428E-AF68-2718FCB88633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21615" yWindow="1335" windowWidth="15375" windowHeight="8325" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AD4268B2-7768-499F-9F38-AFB73F60F5FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>BDR HALL</t>
   </si>
@@ -59,7 +57,10 @@
     <t>Keluar</t>
   </si>
   <si>
-    <t>jumlah</t>
+    <t>Jumlah</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -110,12 +111,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -458,83 +462,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2042D607-C4CF-4B06-A3C3-62AF1890DECA}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
       <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="1"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
       <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="B1:H2"/>
+    <mergeCell ref="B3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>